<commit_message>
Updated data, added .db file, add log_book as pdf
</commit_message>
<xml_diff>
--- a/log book.xlsx
+++ b/log book.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Documents\Kombucha_Brew_Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE3ABE3-C7BF-4148-B0C4-2F9A92963202}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065AAF40-4F51-4369-8C67-6880AECA9281}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{1217B96D-F03A-441C-9008-E755B4774B06}"/>
   </bookViews>
@@ -376,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -412,26 +412,35 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -442,50 +451,37 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -711,7 +707,7 @@
   <dimension ref="A1:W92"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection sqref="A1:T35"/>
+      <selection activeCell="S1" sqref="A1:T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,55 +729,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="25" t="s">
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25" t="s">
+      <c r="L1" s="31"/>
+      <c r="M1" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25" t="s">
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25" t="s">
+      <c r="R1" s="31"/>
+      <c r="S1" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="25"/>
+      <c r="T1" s="31"/>
       <c r="U1" s="18"/>
       <c r="V1" s="18"/>
       <c r="W1" s="18"/>
     </row>
     <row r="2" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="11" t="s">
         <v>37</v>
       </c>
@@ -817,18 +813,18 @@
       <c r="W2" s="17"/>
     </row>
     <row r="3" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="20"/>
       <c r="L3" s="20"/>
       <c r="M3" s="20"/>
@@ -844,42 +840,42 @@
       <c r="W3" s="18"/>
     </row>
     <row r="4" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27" t="s">
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="26" t="s">
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26" t="s">
+      <c r="L4" s="33"/>
+      <c r="M4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26" t="s">
+      <c r="N4" s="33"/>
+      <c r="O4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26" t="s">
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26" t="s">
+      <c r="R4" s="33"/>
+      <c r="S4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="26"/>
+      <c r="T4" s="33"/>
       <c r="U4" s="17"/>
       <c r="V4" s="17"/>
       <c r="W4" s="17"/>
@@ -888,29 +884,29 @@
       <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="34" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
       <c r="U5" s="18"/>
       <c r="V5" s="18"/>
       <c r="W5" s="18"/>
@@ -919,39 +915,39 @@
       <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="33" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26" t="s">
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26" t="s">
+      <c r="L6" s="33"/>
+      <c r="M6" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26" t="s">
+      <c r="N6" s="33"/>
+      <c r="O6" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26" t="s">
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26" t="s">
+      <c r="R6" s="33"/>
+      <c r="S6" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="T6" s="26"/>
+      <c r="T6" s="33"/>
       <c r="U6" s="17"/>
       <c r="V6" s="17"/>
       <c r="W6" s="17"/>
@@ -960,19 +956,19 @@
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="34" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
       <c r="K7" s="14" t="s">
         <v>37</v>
       </c>
@@ -1011,19 +1007,19 @@
       <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="33" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
       <c r="H8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
@@ -1042,39 +1038,39 @@
       <c r="A9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="34" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="25" t="s">
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25" t="s">
+      <c r="L9" s="31"/>
+      <c r="M9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25" t="s">
+      <c r="N9" s="31"/>
+      <c r="O9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25" t="s">
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25" t="s">
+      <c r="R9" s="31"/>
+      <c r="S9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="T9" s="25"/>
+      <c r="T9" s="31"/>
       <c r="U9" s="18"/>
       <c r="V9" s="18"/>
       <c r="W9" s="18"/>
@@ -1083,30 +1079,30 @@
       <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="33" t="s">
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="45"/>
-      <c r="R10" s="45"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="45"/>
-      <c r="U10" s="40"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="24"/>
       <c r="V10" s="17"/>
       <c r="W10" s="17"/>
     </row>
@@ -1114,480 +1110,480 @@
       <c r="A11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="35" t="s">
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="41"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="45"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="45"/>
+      <c r="U11" s="25"/>
       <c r="V11" s="18"/>
       <c r="W11" s="18"/>
     </row>
     <row r="12" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
-      <c r="U12" s="40"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
+      <c r="U12" s="24"/>
       <c r="V12" s="17"/>
       <c r="W12" s="17"/>
     </row>
     <row r="13" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
-      <c r="U13" s="42"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
+      <c r="U13" s="26"/>
       <c r="V13" s="16"/>
       <c r="W13" s="16"/>
     </row>
     <row r="14" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="36" t="s">
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="36"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="36"/>
-      <c r="T14" s="36"/>
-      <c r="U14" s="40"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="24"/>
       <c r="V14" s="17"/>
       <c r="W14" s="17"/>
     </row>
     <row r="15" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="41"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="44"/>
+      <c r="S15" s="44"/>
+      <c r="T15" s="44"/>
+      <c r="U15" s="25"/>
       <c r="V15" s="18"/>
       <c r="W15" s="18"/>
     </row>
     <row r="16" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="26" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="50" t="s">
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="50"/>
-      <c r="S16" s="50"/>
-      <c r="T16" s="50"/>
-      <c r="U16" s="40"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="46"/>
+      <c r="S16" s="46"/>
+      <c r="T16" s="46"/>
+      <c r="U16" s="24"/>
       <c r="V16" s="17"/>
       <c r="W16" s="17"/>
     </row>
     <row r="17" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="51"/>
-      <c r="Q17" s="51"/>
-      <c r="R17" s="51"/>
-      <c r="S17" s="51"/>
-      <c r="T17" s="51"/>
-      <c r="U17" s="41"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="48"/>
+      <c r="Q17" s="48"/>
+      <c r="R17" s="48"/>
+      <c r="S17" s="48"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="25"/>
       <c r="V17" s="18"/>
       <c r="W17" s="18"/>
     </row>
     <row r="18" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="49"/>
-      <c r="Q18" s="49"/>
-      <c r="R18" s="49"/>
-      <c r="S18" s="49"/>
-      <c r="T18" s="49"/>
-      <c r="U18" s="40"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="50"/>
+      <c r="S18" s="50"/>
+      <c r="T18" s="50"/>
+      <c r="U18" s="24"/>
       <c r="V18" s="17"/>
       <c r="W18" s="17"/>
     </row>
     <row r="19" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="51"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="51"/>
-      <c r="U19" s="41"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="48"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="48"/>
+      <c r="S19" s="48"/>
+      <c r="T19" s="48"/>
+      <c r="U19" s="25"/>
       <c r="V19" s="18"/>
       <c r="W19" s="18"/>
     </row>
     <row r="20" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="45"/>
-      <c r="R20" s="45"/>
-      <c r="S20" s="45"/>
-      <c r="T20" s="45"/>
-      <c r="U20" s="40"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="24"/>
       <c r="V20" s="17"/>
       <c r="W20" s="17"/>
     </row>
     <row r="21" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="51"/>
-      <c r="Q21" s="51"/>
-      <c r="R21" s="51"/>
-      <c r="S21" s="51"/>
-      <c r="T21" s="51"/>
-      <c r="U21" s="41"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="25"/>
       <c r="V21" s="18"/>
       <c r="W21" s="18"/>
     </row>
     <row r="22" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="27" t="s">
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="27"/>
-      <c r="T22" s="27"/>
-      <c r="U22" s="40"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="24"/>
       <c r="V22" s="17"/>
       <c r="W22" s="17"/>
     </row>
     <row r="23" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="52"/>
-      <c r="P23" s="52"/>
-      <c r="Q23" s="52"/>
-      <c r="R23" s="46"/>
-      <c r="S23" s="46"/>
-      <c r="T23" s="46"/>
-      <c r="U23" s="41"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="25"/>
       <c r="V23" s="18"/>
       <c r="W23" s="18"/>
     </row>
     <row r="24" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="36" t="s">
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
-      <c r="R24" s="36"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="36"/>
-      <c r="U24" s="40"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="44"/>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="44"/>
+      <c r="S24" s="44"/>
+      <c r="T24" s="44"/>
+      <c r="U24" s="24"/>
       <c r="V24" s="17"/>
       <c r="W24" s="17"/>
     </row>
     <row r="25" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="36"/>
-      <c r="Q25" s="36"/>
-      <c r="R25" s="36"/>
-      <c r="S25" s="36"/>
-      <c r="T25" s="36"/>
-      <c r="U25" s="41"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="44"/>
+      <c r="Q25" s="44"/>
+      <c r="R25" s="44"/>
+      <c r="S25" s="44"/>
+      <c r="T25" s="44"/>
+      <c r="U25" s="25"/>
       <c r="V25" s="18"/>
       <c r="W25" s="18"/>
     </row>
     <row r="26" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-      <c r="Q26" s="27"/>
-      <c r="R26" s="27"/>
-      <c r="S26" s="27"/>
-      <c r="T26" s="27"/>
-      <c r="U26" s="40"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="47"/>
+      <c r="T26" s="47"/>
+      <c r="U26" s="24"/>
       <c r="V26" s="17"/>
       <c r="W26" s="17"/>
     </row>
     <row r="27" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25" t="s">
+      <c r="B27" s="31"/>
+      <c r="C27" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25" t="s">
+      <c r="D27" s="31"/>
+      <c r="E27" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25" t="s">
+      <c r="F27" s="31"/>
+      <c r="G27" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25" t="s">
+      <c r="H27" s="31"/>
+      <c r="I27" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="25"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="27"/>
-      <c r="T27" s="27"/>
-      <c r="U27" s="41"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="47"/>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="47"/>
+      <c r="R27" s="47"/>
+      <c r="S27" s="47"/>
+      <c r="T27" s="47"/>
+      <c r="U27" s="25"/>
       <c r="V27" s="18"/>
       <c r="W27" s="18"/>
     </row>
@@ -1622,17 +1618,17 @@
       <c r="J28" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
-      <c r="R28" s="27"/>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="U28" s="40"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="47"/>
+      <c r="P28" s="47"/>
+      <c r="Q28" s="47"/>
+      <c r="R28" s="47"/>
+      <c r="S28" s="47"/>
+      <c r="T28" s="47"/>
+      <c r="U28" s="24"/>
       <c r="V28" s="17"/>
       <c r="W28" s="17"/>
     </row>
@@ -1647,112 +1643,112 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="43"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
+      <c r="P29" s="47"/>
+      <c r="Q29" s="47"/>
+      <c r="R29" s="47"/>
+      <c r="S29" s="47"/>
+      <c r="T29" s="47"/>
+      <c r="U29" s="27"/>
       <c r="V29" s="21"/>
       <c r="W29" s="21"/>
     </row>
     <row r="30" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26" t="s">
+      <c r="B30" s="33"/>
+      <c r="C30" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26" t="s">
+      <c r="D30" s="33"/>
+      <c r="E30" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26" t="s">
+      <c r="F30" s="33"/>
+      <c r="G30" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26" t="s">
+      <c r="H30" s="33"/>
+      <c r="I30" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="J30" s="26"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="27"/>
-      <c r="R30" s="27"/>
-      <c r="S30" s="27"/>
-      <c r="T30" s="27"/>
-      <c r="U30" s="40"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="47"/>
+      <c r="P30" s="47"/>
+      <c r="Q30" s="47"/>
+      <c r="R30" s="47"/>
+      <c r="S30" s="47"/>
+      <c r="T30" s="47"/>
+      <c r="U30" s="24"/>
       <c r="V30" s="17"/>
       <c r="W30" s="17"/>
     </row>
     <row r="31" spans="1:23" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="27"/>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="27"/>
-      <c r="R31" s="27"/>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
-      <c r="U31" s="43"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="47"/>
+      <c r="O31" s="47"/>
+      <c r="P31" s="47"/>
+      <c r="Q31" s="47"/>
+      <c r="R31" s="47"/>
+      <c r="S31" s="47"/>
+      <c r="T31" s="47"/>
+      <c r="U31" s="27"/>
       <c r="V31" s="21"/>
       <c r="W31" s="21"/>
     </row>
     <row r="32" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26" t="s">
+      <c r="B32" s="33"/>
+      <c r="C32" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26" t="s">
+      <c r="D32" s="33"/>
+      <c r="E32" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26" t="s">
+      <c r="F32" s="33"/>
+      <c r="G32" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26" t="s">
+      <c r="H32" s="33"/>
+      <c r="I32" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="J32" s="26"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="27"/>
-      <c r="R32" s="27"/>
-      <c r="S32" s="27"/>
-      <c r="T32" s="27"/>
-      <c r="U32" s="40"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="47"/>
+      <c r="P32" s="47"/>
+      <c r="Q32" s="47"/>
+      <c r="R32" s="47"/>
+      <c r="S32" s="47"/>
+      <c r="T32" s="47"/>
+      <c r="U32" s="24"/>
       <c r="V32" s="17"/>
       <c r="W32" s="17"/>
     </row>
@@ -1787,17 +1783,17 @@
       <c r="J33" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-      <c r="O33" s="27"/>
-      <c r="P33" s="27"/>
-      <c r="Q33" s="27"/>
-      <c r="R33" s="27"/>
-      <c r="S33" s="27"/>
-      <c r="T33" s="27"/>
-      <c r="U33" s="41"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="47"/>
+      <c r="O33" s="47"/>
+      <c r="P33" s="47"/>
+      <c r="Q33" s="47"/>
+      <c r="R33" s="47"/>
+      <c r="S33" s="47"/>
+      <c r="T33" s="47"/>
+      <c r="U33" s="25"/>
       <c r="V33" s="18"/>
       <c r="W33" s="18"/>
     </row>
@@ -1812,101 +1808,101 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="27"/>
-      <c r="M34" s="27"/>
-      <c r="N34" s="27"/>
-      <c r="O34" s="27"/>
-      <c r="P34" s="27"/>
-      <c r="Q34" s="27"/>
-      <c r="R34" s="27"/>
-      <c r="S34" s="27"/>
-      <c r="T34" s="27"/>
-      <c r="U34" s="43"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="47"/>
+      <c r="P34" s="47"/>
+      <c r="Q34" s="47"/>
+      <c r="R34" s="47"/>
+      <c r="S34" s="47"/>
+      <c r="T34" s="47"/>
+      <c r="U34" s="27"/>
       <c r="V34" s="21"/>
       <c r="W34" s="21"/>
     </row>
     <row r="35" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25" t="s">
+      <c r="B35" s="31"/>
+      <c r="C35" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25" t="s">
+      <c r="D35" s="31"/>
+      <c r="E35" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25" t="s">
+      <c r="F35" s="31"/>
+      <c r="G35" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25" t="s">
+      <c r="H35" s="31"/>
+      <c r="I35" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="J35" s="25"/>
-      <c r="K35" s="27"/>
-      <c r="L35" s="27"/>
-      <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
-      <c r="Q35" s="27"/>
-      <c r="R35" s="27"/>
-      <c r="S35" s="27"/>
-      <c r="T35" s="27"/>
-      <c r="U35" s="41"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="47"/>
+      <c r="Q35" s="47"/>
+      <c r="R35" s="47"/>
+      <c r="S35" s="47"/>
+      <c r="T35" s="47"/>
+      <c r="U35" s="25"/>
       <c r="V35" s="18"/>
       <c r="W35" s="18"/>
     </row>
-    <row r="36" spans="1:23" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
+    <row r="36" spans="1:23" s="22" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
       <c r="K36" s="47"/>
-      <c r="L36" s="48"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="48"/>
-      <c r="O36" s="48"/>
-      <c r="P36" s="48"/>
-      <c r="Q36" s="48"/>
-      <c r="R36" s="48"/>
-      <c r="S36" s="48"/>
-      <c r="T36" s="48"/>
-      <c r="U36" s="43"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="47"/>
+      <c r="N36" s="47"/>
+      <c r="O36" s="47"/>
+      <c r="P36" s="47"/>
+      <c r="Q36" s="47"/>
+      <c r="R36" s="47"/>
+      <c r="S36" s="47"/>
+      <c r="T36" s="47"/>
+      <c r="U36" s="27"/>
       <c r="V36" s="21"/>
       <c r="W36" s="21"/>
     </row>
     <row r="37" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="47"/>
+      <c r="L37" s="47"/>
+      <c r="M37" s="47"/>
+      <c r="N37" s="47"/>
+      <c r="O37" s="47"/>
+      <c r="P37" s="47"/>
+      <c r="Q37" s="47"/>
+      <c r="R37" s="47"/>
+      <c r="S37" s="47"/>
+      <c r="T37" s="47"/>
     </row>
     <row r="38" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
@@ -2580,7 +2576,6 @@
   </sheetData>
   <mergeCells count="136">
     <mergeCell ref="K24:T25"/>
-    <mergeCell ref="K26:T35"/>
     <mergeCell ref="N23:Q23"/>
     <mergeCell ref="P18:T18"/>
     <mergeCell ref="P19:T19"/>
@@ -2590,6 +2585,7 @@
     <mergeCell ref="K19:O19"/>
     <mergeCell ref="K20:O20"/>
     <mergeCell ref="K21:O21"/>
+    <mergeCell ref="K26:T37"/>
     <mergeCell ref="K11:T13"/>
     <mergeCell ref="K14:T15"/>
     <mergeCell ref="K16:O16"/>
@@ -2700,6 +2696,11 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="E35:F35"/>
@@ -2710,13 +2711,8 @@
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="I36:J36"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.23284313725490197" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.23284313725490197" top="0.75" bottom="0.30637254901960786" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;C&amp;"-,Bold"&amp;20Kombucha </oddHeader>

</xml_diff>